<commit_message>
Update LJH : 일정 수정
</commit_message>
<xml_diff>
--- a/2019년 Project 일정.xlsx
+++ b/2019년 Project 일정.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9563F4D-4300-4797-96BC-F403A6FA8914}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE60DD2-E60B-4251-BBA6-941B5481B2DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,16 +283,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. 광학계 검토
-2. 프로젝트 시작 (3/11)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 광학계 검토 (2/13)
 2. 프로젝트 시작 (3/5)
 3. Mobis 미팅(3/7) : 비젼 미팅
    전체 일정 지연 예상
 4. 광학계 검토 (3/12)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 광학계 검토(3/11)
+2. 프로젝트 시작 (3/11)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1911,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2041,10 +2041,10 @@
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update LJH : 2019년 Project 일정
</commit_message>
<xml_diff>
--- a/2019년 Project 일정.xlsx
+++ b/2019년 Project 일정.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE60DD2-E60B-4251-BBA6-941B5481B2DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E347579E-78D2-4C65-96D7-5F94D1E63CB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1364,6 +1364,89 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA75B060-866B-453B-B007-234EC51E820B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10287000" y="853109"/>
+          <a:ext cx="2584174" cy="2617304"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="22225" cap="rnd">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="4400">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Delay</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1912,7 +1995,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>